<commit_message>
stock buy and sell leetcode blind75
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\the-ab-repositories\DSA-Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BA18C2-0C15-4088-BC8A-F7B69D93BD7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEF3E13-336D-488B-95C0-BA62292EE2AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
   <si>
     <t>Array</t>
   </si>
@@ -633,13 +633,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +653,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -661,12 +661,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -674,7 +677,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -682,407 +685,407 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="82" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" ht="102" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="203" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="41" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="41" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
maximum product subarray blind75
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\the-ab-repositories\DSA-Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A1F3F8-B0AB-4F3E-AC04-A8E1AE5977AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75558DDC-2822-4E76-8C23-ED0FDD6E4303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
   <si>
     <t>Array</t>
   </si>
@@ -292,13 +292,16 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Revised other people's submissions?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +319,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -342,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -350,6 +361,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -631,15 +643,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="20.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,8 +664,11 @@
       <c r="D1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -661,7 +676,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -669,7 +684,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -677,7 +692,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -685,7 +700,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -693,402 +708,405 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="20.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="102" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="82" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" ht="203" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="41" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" ht="116" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" ht="41" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" ht="116" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="144" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" ht="145" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" ht="20.5" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
min in rotated sorted array - blind75:
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\the-ab-repositories\DSA-Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75558DDC-2822-4E76-8C23-ED0FDD6E4303}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970D7E40-A7E6-4ADB-902B-1DB7DC9456D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="90">
   <si>
     <t>Array</t>
   </si>
@@ -646,7 +646,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -719,6 +719,9 @@
     <row r="8" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
search in rotated array -blind75
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\the-ab-repositories\DSA-Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970D7E40-A7E6-4ADB-902B-1DB7DC9456D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ECEE9D-50F5-4C95-BF69-96CC0645B60F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
   <si>
     <t>Array</t>
   </si>
@@ -646,7 +646,7 @@
   <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -727,6 +727,9 @@
     <row r="9" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
dp climbing stairs + cache
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\the-ab-repositories\DSA-Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5D7630-EDD6-4C7C-8764-8FD1B296A23C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80423888-470A-4BC6-8B59-28C5E96A3EF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>Array</t>
   </si>
@@ -657,13 +657,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="61.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -686,7 +686,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>87</v>
       </c>
@@ -697,7 +697,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>87</v>
       </c>
@@ -708,7 +708,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>87</v>
       </c>
@@ -719,7 +719,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>87</v>
       </c>
@@ -730,7 +730,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>87</v>
       </c>
@@ -741,7 +741,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>87</v>
       </c>
@@ -752,7 +752,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>87</v>
       </c>
@@ -763,7 +763,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>87</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>87</v>
       </c>
@@ -791,7 +791,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>87</v>
       </c>
@@ -802,7 +802,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="20.5" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
@@ -810,7 +810,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>87</v>
       </c>
@@ -821,7 +821,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>87</v>
       </c>
@@ -832,7 +832,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>87</v>
       </c>
@@ -843,7 +843,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>87</v>
       </c>
@@ -854,7 +854,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>87</v>
       </c>
@@ -865,7 +865,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="24" spans="2:6" ht="102" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="82" x14ac:dyDescent="0.35">
       <c r="C24" s="1" t="s">
         <v>17</v>
       </c>
@@ -873,7 +873,10 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
@@ -881,7 +884,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C26" s="2" t="s">
         <v>19</v>
       </c>
@@ -889,7 +892,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C27" s="2" t="s">
         <v>20</v>
       </c>
@@ -897,7 +900,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
@@ -905,7 +908,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C29" s="2" t="s">
         <v>22</v>
       </c>
@@ -913,7 +916,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C30" s="2" t="s">
         <v>23</v>
       </c>
@@ -921,7 +924,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C31" s="2" t="s">
         <v>24</v>
       </c>
@@ -929,7 +932,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C32" s="2" t="s">
         <v>25</v>
       </c>
@@ -937,7 +940,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C33" s="2" t="s">
         <v>26</v>
       </c>
@@ -945,7 +948,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C34" s="2" t="s">
         <v>27</v>
       </c>
@@ -953,7 +956,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C35" s="2" t="s">
         <v>28</v>
       </c>
@@ -961,7 +964,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="39" spans="3:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:6" ht="20.5" x14ac:dyDescent="0.35">
       <c r="C39" s="1" t="s">
         <v>29</v>
       </c>
@@ -969,7 +972,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C40" s="2" t="s">
         <v>30</v>
       </c>
@@ -977,7 +980,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C41" s="2" t="s">
         <v>31</v>
       </c>
@@ -985,7 +988,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C42" s="2" t="s">
         <v>32</v>
       </c>
@@ -993,7 +996,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C43" s="2" t="s">
         <v>33</v>
       </c>
@@ -1001,7 +1004,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C44" s="2" t="s">
         <v>34</v>
       </c>
@@ -1009,7 +1012,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="C45" s="2" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +1020,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="C46" s="2" t="s">
         <v>36</v>
       </c>
@@ -1025,7 +1028,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="3:6" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:6" ht="203" x14ac:dyDescent="0.35">
       <c r="C47" s="2" t="s">
         <v>37</v>
       </c>
@@ -1033,7 +1036,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="51" spans="3:6" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:6" ht="41" x14ac:dyDescent="0.35">
       <c r="C51" s="1" t="s">
         <v>38</v>
       </c>
@@ -1041,7 +1044,7 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C52" s="2" t="s">
         <v>39</v>
       </c>
@@ -1049,7 +1052,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C53" s="2" t="s">
         <v>40</v>
       </c>
@@ -1057,7 +1060,7 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C54" s="2" t="s">
         <v>41</v>
       </c>
@@ -1065,7 +1068,7 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="C55" s="2" t="s">
         <v>42</v>
       </c>
@@ -1073,7 +1076,7 @@
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:6" ht="116" x14ac:dyDescent="0.35">
       <c r="C56" s="2" t="s">
         <v>43</v>
       </c>
@@ -1081,7 +1084,7 @@
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="60" spans="3:6" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:6" ht="41" x14ac:dyDescent="0.35">
       <c r="C60" s="1" t="s">
         <v>44</v>
       </c>
@@ -1089,7 +1092,7 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C61" s="2" t="s">
         <v>45</v>
       </c>
@@ -1097,7 +1100,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C62" s="2" t="s">
         <v>46</v>
       </c>
@@ -1105,7 +1108,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C63" s="2" t="s">
         <v>47</v>
       </c>
@@ -1113,7 +1116,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C64" s="2" t="s">
         <v>48</v>
       </c>
@@ -1121,7 +1124,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C65" s="2" t="s">
         <v>49</v>
       </c>
@@ -1129,7 +1132,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C66" s="2" t="s">
         <v>50</v>
       </c>
@@ -1137,7 +1140,7 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="70" spans="3:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:6" ht="20.5" x14ac:dyDescent="0.35">
       <c r="C70" s="1" t="s">
         <v>51</v>
       </c>
@@ -1145,7 +1148,7 @@
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C71" s="2" t="s">
         <v>52</v>
       </c>
@@ -1153,7 +1156,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C72" s="2" t="s">
         <v>53</v>
       </c>
@@ -1161,7 +1164,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C73" s="2" t="s">
         <v>54</v>
       </c>
@@ -1169,7 +1172,7 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C74" s="2" t="s">
         <v>55</v>
       </c>
@@ -1177,7 +1180,7 @@
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="78" spans="3:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:6" ht="20.5" x14ac:dyDescent="0.35">
       <c r="C78" s="1" t="s">
         <v>56</v>
       </c>
@@ -1185,7 +1188,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="3:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="C79" s="2" t="s">
         <v>57</v>
       </c>
@@ -1193,7 +1196,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="C80" s="2" t="s">
         <v>58</v>
       </c>
@@ -1201,7 +1204,7 @@
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C81" s="2" t="s">
         <v>59</v>
       </c>
@@ -1209,7 +1212,7 @@
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C82" s="2" t="s">
         <v>60</v>
       </c>
@@ -1217,7 +1220,7 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C83" s="2" t="s">
         <v>61</v>
       </c>
@@ -1225,7 +1228,7 @@
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C84" s="2" t="s">
         <v>62</v>
       </c>
@@ -1233,7 +1236,7 @@
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C85" s="2" t="s">
         <v>63</v>
       </c>
@@ -1241,7 +1244,7 @@
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C86" s="2" t="s">
         <v>64</v>
       </c>
@@ -1249,7 +1252,7 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C87" s="2" t="s">
         <v>65</v>
       </c>
@@ -1257,7 +1260,7 @@
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="3:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:6" ht="116" x14ac:dyDescent="0.35">
       <c r="C88" s="2" t="s">
         <v>66</v>
       </c>
@@ -1265,7 +1268,7 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="92" spans="3:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:6" ht="20.5" x14ac:dyDescent="0.35">
       <c r="C92" s="1" t="s">
         <v>67</v>
       </c>
@@ -1273,7 +1276,7 @@
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C93" s="2" t="s">
         <v>68</v>
       </c>
@@ -1281,7 +1284,7 @@
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C94" s="2" t="s">
         <v>69</v>
       </c>
@@ -1289,7 +1292,7 @@
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C95" s="2" t="s">
         <v>70</v>
       </c>
@@ -1297,7 +1300,7 @@
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C96" s="2" t="s">
         <v>71</v>
       </c>
@@ -1305,7 +1308,7 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C97" s="2" t="s">
         <v>72</v>
       </c>
@@ -1313,7 +1316,7 @@
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C98" s="2" t="s">
         <v>73</v>
       </c>
@@ -1321,7 +1324,7 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C99" s="2" t="s">
         <v>74</v>
       </c>
@@ -1329,7 +1332,7 @@
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="3:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:6" ht="145" x14ac:dyDescent="0.35">
       <c r="C100" s="2" t="s">
         <v>75</v>
       </c>
@@ -1337,7 +1340,7 @@
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C101" s="2" t="s">
         <v>76</v>
       </c>
@@ -1345,7 +1348,7 @@
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
     </row>
-    <row r="102" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C102" s="2" t="s">
         <v>77</v>
       </c>
@@ -1353,7 +1356,7 @@
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C103" s="2" t="s">
         <v>78</v>
       </c>
@@ -1361,7 +1364,7 @@
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C104" s="2" t="s">
         <v>79</v>
       </c>
@@ -1369,7 +1372,7 @@
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C105" s="2" t="s">
         <v>80</v>
       </c>
@@ -1377,7 +1380,7 @@
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
     </row>
-    <row r="106" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C106" s="2" t="s">
         <v>81</v>
       </c>
@@ -1385,7 +1388,7 @@
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
     </row>
-    <row r="110" spans="3:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:6" ht="20.5" x14ac:dyDescent="0.35">
       <c r="C110" s="1" t="s">
         <v>82</v>
       </c>
@@ -1393,7 +1396,7 @@
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C111" s="2" t="s">
         <v>48</v>
       </c>
@@ -1401,7 +1404,7 @@
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
     </row>
-    <row r="112" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C112" s="2" t="s">
         <v>83</v>
       </c>
@@ -1409,7 +1412,7 @@
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
     </row>
-    <row r="113" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C113" s="2" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
house robber 2 marked excel
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\the-ab-repositories\DSA-Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0649336C-5603-47D5-8897-B5F8E6717EC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16A60B7-8D5B-4257-97E9-BA25B077958D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="93">
   <si>
     <t>Array</t>
   </si>
@@ -658,7 +658,7 @@
   <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,6 +942,9 @@
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
       <c r="C32" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
max depth binary tree
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="93">
   <si>
     <t xml:space="preserve">Difficulty</t>
   </si>
@@ -678,8 +678,8 @@
   </sheetPr>
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G93" activeCellId="0" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1349,6 +1349,9 @@
       <c r="F92" s="2"/>
     </row>
     <row r="93" customFormat="false" ht="86.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C93" s="4" t="s">
         <v>76</v>
       </c>
@@ -1357,6 +1360,9 @@
       <c r="F93" s="4"/>
     </row>
     <row r="94" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C94" s="4" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
build tree using preorder inorder
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
   <si>
     <t xml:space="preserve">Difficulty</t>
   </si>
@@ -678,8 +678,8 @@
   </sheetPr>
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A95" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A98" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B101" activeCellId="0" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1390,7 +1390,7 @@
       <c r="F96" s="4"/>
     </row>
     <row r="97" customFormat="false" ht="86.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C97" s="4" t="s">
@@ -1409,7 +1409,7 @@
       <c r="F98" s="4"/>
     </row>
     <row r="99" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C99" s="4" t="s">
@@ -1428,6 +1428,9 @@
       <c r="F100" s="4"/>
     </row>
     <row r="101" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C101" s="4" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
set to zero in matrix
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="93">
   <si>
     <t xml:space="preserve">Difficulty</t>
   </si>
@@ -678,8 +678,8 @@
   </sheetPr>
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B104" activeCellId="0" sqref="B104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B71" activeCellId="0" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1221,6 +1221,9 @@
       <c r="F70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C71" s="4" t="s">
         <v>60</v>
       </c>
@@ -1464,7 +1467,7 @@
       <c r="F103" s="4"/>
     </row>
     <row r="104" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="0" t="s">
+      <c r="B104" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C104" s="4" t="s">

</xml_diff>

<commit_message>
substring count + longest substrings
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
   <si>
     <t xml:space="preserve">Difficulty</t>
   </si>
@@ -678,8 +678,8 @@
   </sheetPr>
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B80" activeCellId="0" sqref="B80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C86" activeCellId="0" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1275,7 +1275,7 @@
       <c r="F79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="100.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
+      <c r="B80" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C80" s="4" t="s">
@@ -1305,6 +1305,9 @@
       <c r="F82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C83" s="4" t="s">
         <v>69</v>
       </c>
@@ -1313,6 +1316,9 @@
       <c r="F83" s="4"/>
     </row>
     <row r="84" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C84" s="4" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
word search initial approach
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
   <si>
     <t xml:space="preserve">Difficulty</t>
   </si>
@@ -679,7 +679,7 @@
   <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F72" activeCellId="0" sqref="F72"/>
+      <selection pane="topLeft" activeCell="H73" activeCellId="0" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1232,7 +1232,7 @@
       <c r="F71" s="4"/>
     </row>
     <row r="72" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C72" s="4" t="s">
@@ -1243,6 +1243,9 @@
       <c r="F72" s="4"/>
     </row>
     <row r="73" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C73" s="4" t="s">
         <v>62</v>
       </c>
@@ -1341,7 +1344,7 @@
       <c r="F85" s="4"/>
     </row>
     <row r="86" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C86" s="4" t="s">
@@ -1352,7 +1355,7 @@
       <c r="F86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="0" t="s">
+      <c r="B87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C87" s="4" t="s">

</xml_diff>

<commit_message>
top k freq items
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="93">
   <si>
     <t xml:space="preserve">Difficulty</t>
   </si>
@@ -293,9 +293,6 @@
   </si>
   <si>
     <t xml:space="preserve">Heap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maybe</t>
   </si>
   <si>
     <t xml:space="preserve">Top K Frequent Elements</t>
@@ -681,8 +678,8 @@
   </sheetPr>
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F112" activeCellId="0" sqref="F112"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A107" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B112" activeCellId="0" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1030,7 +1027,7 @@
       <c r="F39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -1301,7 +1298,7 @@
       <c r="F80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="86.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="0" t="s">
+      <c r="B81" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C81" s="4" t="s">
@@ -1544,8 +1541,8 @@
       <c r="F110" s="2"/>
     </row>
     <row r="111" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="0" t="s">
-        <v>91</v>
+      <c r="B111" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>56</v>
@@ -1555,8 +1552,11 @@
       <c r="F111" s="4"/>
     </row>
     <row r="112" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C112" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="113" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C113" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>

</xml_diff>

<commit_message>
Pacific Atlantic Waterflow solution excel edit
</commit_message>
<xml_diff>
--- a/Blind75.xlsx
+++ b/Blind75.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="93">
   <si>
     <t xml:space="preserve">Difficulty</t>
   </si>
@@ -679,7 +679,7 @@
   <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
+      <selection pane="topLeft" activeCell="D43" activeCellId="0" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1038,7 +1038,7 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -1049,6 +1049,9 @@
       <c r="F41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>40</v>
       </c>

</xml_diff>